<commit_message>
feat(batchgen): update the format of the excel table
1. Update the format of the excel table.
2. Add the new tool 'batchrun' (coding on-going).
</commit_message>
<xml_diff>
--- a/example/reg_table.xlsx
+++ b/example/reg_table.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">FileName</t>
   </si>
   <si>
+    <t xml:space="preserve">PAT-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eng.</t>
   </si>
   <si>
@@ -41,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">Metion2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaseAddr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metion3</t>
   </si>
   <si>
     <t xml:space="preserve">PatternStatus</t>
@@ -100,6 +109,9 @@
 bus reg1</t>
   </si>
   <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xc8</t>
   </si>
   <si>
@@ -110,6 +122,9 @@
 bus reg2</t>
   </si>
   <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x8</t>
   </si>
   <si>
@@ -125,6 +140,9 @@
     <t xml:space="preserve">GROUP2_ADDR_VAR1</t>
   </si>
   <si>
+    <t xml:space="preserve">A8A8AA88</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xc</t>
   </si>
   <si>
@@ -146,10 +164,16 @@
     <t xml:space="preserve">GROUP2_VAR2_UNSIGNED</t>
   </si>
   <si>
+    <t xml:space="preserve">1E</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xffec</t>
   </si>
   <si>
     <t xml:space="preserve">GROUP2_VAR2_SIGNED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFEC</t>
   </si>
   <si>
     <t xml:space="preserve">0x18</t>
@@ -186,10 +210,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
     </font>
@@ -209,47 +233,41 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Noto Sans CJK TC"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF808080"/>
       <name val="Noto Sans CJK TC"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -332,128 +350,160 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,276 +579,537 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1f497d"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="eeece1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4f81bd"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="c0504d"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9bbb59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064a2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4bacc6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="f79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ff"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="7.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.05"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="3" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" s="17" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" s="20" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" s="24" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="D9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="E9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="F9" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" s="17" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" s="20" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="F10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="11" s="24" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="E11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+    <row r="12" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="D12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="E12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="F12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="13" t="s">
+    </row>
+    <row r="13" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="23" t="s">
+      <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="C13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="18" t="s">
+      <c r="E15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>50</v>
-      </c>
+      <c r="E17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>